<commit_message>
Update inventory data - 2025-07-04 06:42:56
</commit_message>
<xml_diff>
--- a/inventory_data.xlsx
+++ b/inventory_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="70">
   <si>
     <t>Location</t>
   </si>
@@ -40,28 +40,34 @@
     <t>C2</t>
   </si>
   <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
     <t>C1</t>
   </si>
   <si>
     <t>B3</t>
   </si>
   <si>
-    <t>E4</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>A2</t>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
   </si>
   <si>
     <t>Stuff</t>
@@ -70,6 +76,33 @@
     <t>UX100</t>
   </si>
   <si>
+    <t>Touchstone Stuff</t>
+  </si>
+  <si>
+    <t>Mayfield Stuff</t>
+  </si>
+  <si>
+    <t>Omni-Tract Stuff</t>
+  </si>
+  <si>
+    <t>BNS RF Lesion Generator for Neurosurgery</t>
+  </si>
+  <si>
+    <t>Codman Electrosurgical Generator</t>
+  </si>
+  <si>
+    <t>Elliquence Surgi-Max Plus</t>
+  </si>
+  <si>
+    <t>Integra Duo Headlight &amp; Accessory</t>
+  </si>
+  <si>
+    <t>Lextec Lightsource</t>
+  </si>
+  <si>
+    <t>BNS 4-Channel RF Lesion Generator</t>
+  </si>
+  <si>
     <t>Codman Certas Plus</t>
   </si>
   <si>
@@ -85,31 +118,28 @@
     <t>Integra Luxtec Lightsource</t>
   </si>
   <si>
-    <t>Touchstone Stuff</t>
-  </si>
-  <si>
-    <t>BNS 4-Channel RF Lesion Generator</t>
-  </si>
-  <si>
-    <t>BNS RF Lesion Generator for Neurosurgery</t>
-  </si>
-  <si>
-    <t>Mayfield Stuff</t>
-  </si>
-  <si>
-    <t>Omni-Tract Stuff</t>
-  </si>
-  <si>
-    <t>Codman Electrosurgical Generator</t>
-  </si>
-  <si>
-    <t>Elliquence Surgi-Max Plus</t>
-  </si>
-  <si>
-    <t>Integra Duo Headlight &amp; Accessory</t>
-  </si>
-  <si>
-    <t>Lextec Lightsource</t>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>New Item</t>
+  </si>
+  <si>
+    <t>RFE2-C</t>
+  </si>
+  <si>
+    <t>901001ESUO</t>
+  </si>
+  <si>
+    <t>IEC4-SP</t>
+  </si>
+  <si>
+    <t>90600</t>
+  </si>
+  <si>
+    <t>00MLX</t>
+  </si>
+  <si>
+    <t>RFE4-B</t>
   </si>
   <si>
     <t>82-8852</t>
@@ -124,24 +154,6 @@
     <t>144733</t>
   </si>
   <si>
-    <t>00MLX</t>
-  </si>
-  <si>
-    <t>RFE4-B</t>
-  </si>
-  <si>
-    <t>RFE2-C</t>
-  </si>
-  <si>
-    <t>901001ESUO</t>
-  </si>
-  <si>
-    <t>IEC4-SP</t>
-  </si>
-  <si>
-    <t>90600</t>
-  </si>
-  <si>
     <t>2150601326</t>
   </si>
   <si>
@@ -178,6 +190,33 @@
     <t>STH Trade-in, Dead motherboard</t>
   </si>
   <si>
+    <t>https://www.saturdayeveningpost.com/wp-content/uploads/satevepost/2019-12-19-random-stuff-860x573.jpg</t>
+  </si>
+  <si>
+    <t>https://media-ecn.s3.amazonaws.com/embedded_image/2016/02/fda.jpg</t>
+  </si>
+  <si>
+    <t>https://products.integralife.com/ccstore/v1/images/?source=/file/products/Omni-Tract%20Flexible%20Wishbone%20Urologic%20Surgery%20Retractor%20System%20OS%201%20Image.png</t>
+  </si>
+  <si>
+    <t>https://www.bnsmed.com/data/watermark/20200924/5f6c31aea1382.jpg</t>
+  </si>
+  <si>
+    <t>https://products.integralife.com/ccstore/v1/images/?source=/file/products/Codman%20Electrosurgical%20Generator%20OS%201%20Image.jpg</t>
+  </si>
+  <si>
+    <t>https://www.elliquence.com/wp-content/uploads/2016/01/Surgi-Max-Plus-Device.jpg</t>
+  </si>
+  <si>
+    <t>https://www.aamedicalstore.com/SSP Applications/AA Medical SCA/AA Medical/img/Product Images/Integra-Duo-LED-Headlight-Set_01.JPG</t>
+  </si>
+  <si>
+    <t>https://products.integralife.com/ccstore/v1/images/?source=/file/v6400991064904479991/products/MLX-300-Xenon-Lightsources.jpg</t>
+  </si>
+  <si>
+    <t>https://www.bnsmed.com/data/watermark/20200924/5f6c30bda627b.jpg</t>
+  </si>
+  <si>
     <t>https://products.integralife.com/ccstore/v1/images/?source=/file/v3841902670343812321/products/ETK_01.png</t>
   </si>
   <si>
@@ -185,33 +224,6 @@
   </si>
   <si>
     <t>https://products.integralife.com/ccstore/v1/images/?source=/file/v5137398853523069574/products/823190.jpg</t>
-  </si>
-  <si>
-    <t>https://products.integralife.com/ccstore/v1/images/?source=/file/v6400991064904479991/products/MLX-300-Xenon-Lightsources.jpg</t>
-  </si>
-  <si>
-    <t>https://www.saturdayeveningpost.com/wp-content/uploads/satevepost/2019-12-19-random-stuff-860x573.jpg</t>
-  </si>
-  <si>
-    <t>https://www.bnsmed.com/data/watermark/20200924/5f6c30bda627b.jpg</t>
-  </si>
-  <si>
-    <t>https://www.bnsmed.com/data/watermark/20200924/5f6c31aea1382.jpg</t>
-  </si>
-  <si>
-    <t>https://media-ecn.s3.amazonaws.com/embedded_image/2016/02/fda.jpg</t>
-  </si>
-  <si>
-    <t>https://products.integralife.com/ccstore/v1/images/?source=/file/products/Omni-Tract%20Flexible%20Wishbone%20Urologic%20Surgery%20Retractor%20System%20OS%201%20Image.png</t>
-  </si>
-  <si>
-    <t>https://products.integralife.com/ccstore/v1/images/?source=/file/products/Codman%20Electrosurgical%20Generator%20OS%201%20Image.jpg</t>
-  </si>
-  <si>
-    <t>https://www.elliquence.com/wp-content/uploads/2016/01/Surgi-Max-Plus-Device.jpg</t>
-  </si>
-  <si>
-    <t>https://www.aamedicalstore.com/SSP Applications/AA Medical SCA/AA Medical/img/Product Images/Integra-Duo-LED-Headlight-Set_01.JPG</t>
   </si>
 </sst>
 </file>
@@ -588,7 +600,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -631,7 +643,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -642,13 +654,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -656,196 +668,148 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" t="s">
-        <v>48</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" t="s">
-        <v>49</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s">
-        <v>50</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
       <c r="G12" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
@@ -853,70 +817,97 @@
       <c r="C13">
         <v>1</v>
       </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
       <c r="G13" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="F14" t="s">
+        <v>52</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
+        <v>53</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>54</v>
+      </c>
       <c r="G16" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" t="s">
+        <v>54</v>
+      </c>
       <c r="G17" s="2" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -924,16 +915,22 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>44</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" t="s">
+        <v>54</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -941,16 +938,22 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>45</v>
+      </c>
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" t="s">
+        <v>55</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -958,7 +961,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -966,22 +969,34 @@
       <c r="D20" t="s">
         <v>40</v>
       </c>
+      <c r="E20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" t="s">
+        <v>56</v>
+      </c>
       <c r="G20" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="E21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" t="s">
+        <v>57</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>65</v>
@@ -992,16 +1007,57 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" t="s">
-        <v>36</v>
-      </c>
       <c r="G22" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update inventory data - 2025-07-04 06:44:10
</commit_message>
<xml_diff>
--- a/inventory_data.xlsx
+++ b/inventory_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
   <si>
     <t>Location</t>
   </si>
@@ -64,12 +64,6 @@
     <t>B3</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
     <t>Stuff</t>
   </si>
   <si>
@@ -116,12 +110,6 @@
   </si>
   <si>
     <t>Integra Luxtec Lightsource</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>New Item</t>
   </si>
   <si>
     <t>RFE2-C</t>
@@ -600,7 +588,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -643,7 +631,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -654,13 +642,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -668,13 +656,13 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -682,13 +670,13 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -696,13 +684,13 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -710,16 +698,16 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -727,16 +715,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -744,16 +732,16 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -761,16 +749,16 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -778,16 +766,16 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -795,16 +783,16 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -812,16 +800,16 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -829,19 +817,19 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -849,19 +837,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -869,22 +857,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -892,22 +880,22 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -915,22 +903,22 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" t="s">
         <v>44</v>
       </c>
-      <c r="E18" t="s">
-        <v>48</v>
-      </c>
       <c r="F18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -938,22 +926,22 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
         <v>45</v>
       </c>
-      <c r="E19" t="s">
-        <v>49</v>
-      </c>
       <c r="F19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -961,22 +949,22 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F20" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -984,22 +972,22 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1007,57 +995,13 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update inventory data - 2025-07-04 06:44:37
</commit_message>
<xml_diff>
--- a/inventory_data.xlsx
+++ b/inventory_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
   <si>
     <t>Location</t>
   </si>
@@ -37,79 +37,88 @@
     <t>Image_URL</t>
   </si>
   <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
     <t>C2</t>
   </si>
   <si>
-    <t>E4</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>B3</t>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Touchstone Stuff</t>
+  </si>
+  <si>
+    <t>Mayfield Stuff</t>
+  </si>
+  <si>
+    <t>Omni-Tract Stuff</t>
+  </si>
+  <si>
+    <t>BNS RF Lesion Generator for Neurosurgery</t>
+  </si>
+  <si>
+    <t>Codman Electrosurgical Generator</t>
+  </si>
+  <si>
+    <t>Elliquence Surgi-Max Plus</t>
+  </si>
+  <si>
+    <t>Integra Duo Headlight &amp; Accessory</t>
+  </si>
+  <si>
+    <t>Lextec Lightsource</t>
+  </si>
+  <si>
+    <t>BNS 4-Channel RF Lesion Generator</t>
+  </si>
+  <si>
+    <t>Codman Certas Plus</t>
+  </si>
+  <si>
+    <t>Codman Licox PtO2 Monitor</t>
+  </si>
+  <si>
+    <t>Codman Medos Valve Programmer</t>
+  </si>
+  <si>
+    <t>Integra LicocCMP Tissue Oxygen Pressure Monitor</t>
+  </si>
+  <si>
+    <t>Integra Luxtec Lightsource</t>
   </si>
   <si>
     <t>Stuff</t>
   </si>
   <si>
+    <t>Test</t>
+  </si>
+  <si>
     <t>UX100</t>
   </si>
   <si>
-    <t>Touchstone Stuff</t>
-  </si>
-  <si>
-    <t>Mayfield Stuff</t>
-  </si>
-  <si>
-    <t>Omni-Tract Stuff</t>
-  </si>
-  <si>
-    <t>BNS RF Lesion Generator for Neurosurgery</t>
-  </si>
-  <si>
-    <t>Codman Electrosurgical Generator</t>
-  </si>
-  <si>
-    <t>Elliquence Surgi-Max Plus</t>
-  </si>
-  <si>
-    <t>Integra Duo Headlight &amp; Accessory</t>
-  </si>
-  <si>
-    <t>Lextec Lightsource</t>
-  </si>
-  <si>
-    <t>BNS 4-Channel RF Lesion Generator</t>
-  </si>
-  <si>
-    <t>Codman Certas Plus</t>
-  </si>
-  <si>
-    <t>Codman Licox PtO2 Monitor</t>
-  </si>
-  <si>
-    <t>Codman Medos Valve Programmer</t>
-  </si>
-  <si>
-    <t>Integra LicocCMP Tissue Oxygen Pressure Monitor</t>
-  </si>
-  <si>
-    <t>Integra Luxtec Lightsource</t>
+    <t>New Item</t>
   </si>
   <si>
     <t>RFE2-C</t>
@@ -588,7 +597,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -631,52 +640,58 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
       <c r="G5" s="2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -684,30 +699,33 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
       <c r="G6" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -715,16 +733,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -732,16 +750,16 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -749,16 +767,16 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -766,16 +784,16 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -789,10 +807,13 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -800,21 +821,24 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>41</v>
+      </c>
+      <c r="F13" t="s">
+        <v>52</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
@@ -823,38 +847,44 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>43</v>
+      </c>
+      <c r="E15" t="s">
+        <v>46</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
         <v>28</v>
@@ -863,21 +893,21 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
@@ -886,44 +916,44 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F17" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F18" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
         <v>30</v>
@@ -932,13 +962,13 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F19" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>64</v>
@@ -954,17 +984,8 @@
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" t="s">
-        <v>52</v>
-      </c>
       <c r="G20" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -972,22 +993,10 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C21">
         <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -995,36 +1004,58 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
         <v>16</v>
       </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>54</v>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G4" r:id="rId1"/>
-    <hyperlink ref="G5" r:id="rId2"/>
-    <hyperlink ref="G6" r:id="rId3"/>
-    <hyperlink ref="G7" r:id="rId4"/>
-    <hyperlink ref="G8" r:id="rId5"/>
-    <hyperlink ref="G9" r:id="rId6"/>
-    <hyperlink ref="G10" r:id="rId7"/>
-    <hyperlink ref="G11" r:id="rId8"/>
-    <hyperlink ref="G12" r:id="rId9"/>
-    <hyperlink ref="G13" r:id="rId10"/>
-    <hyperlink ref="G14" r:id="rId11"/>
-    <hyperlink ref="G15" r:id="rId12"/>
-    <hyperlink ref="G16" r:id="rId13"/>
-    <hyperlink ref="G17" r:id="rId14"/>
-    <hyperlink ref="G18" r:id="rId15"/>
-    <hyperlink ref="G19" r:id="rId16"/>
-    <hyperlink ref="G20" r:id="rId17"/>
-    <hyperlink ref="G21" r:id="rId18"/>
-    <hyperlink ref="G22" r:id="rId19"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
+    <hyperlink ref="G7" r:id="rId6"/>
+    <hyperlink ref="G8" r:id="rId7"/>
+    <hyperlink ref="G9" r:id="rId8"/>
+    <hyperlink ref="G10" r:id="rId9"/>
+    <hyperlink ref="G11" r:id="rId10"/>
+    <hyperlink ref="G12" r:id="rId11"/>
+    <hyperlink ref="G13" r:id="rId12"/>
+    <hyperlink ref="G14" r:id="rId13"/>
+    <hyperlink ref="G15" r:id="rId14"/>
+    <hyperlink ref="G16" r:id="rId15"/>
+    <hyperlink ref="G17" r:id="rId16"/>
+    <hyperlink ref="G18" r:id="rId17"/>
+    <hyperlink ref="G19" r:id="rId18"/>
+    <hyperlink ref="G20" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update inventory data - 2025-07-04 06:44:55
</commit_message>
<xml_diff>
--- a/inventory_data.xlsx
+++ b/inventory_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="69">
   <si>
     <t>Location</t>
   </si>
@@ -37,6 +37,9 @@
     <t>Image_URL</t>
   </si>
   <si>
+    <t>C2</t>
+  </si>
+  <si>
     <t>E4</t>
   </si>
   <si>
@@ -61,10 +64,13 @@
     <t>B3</t>
   </si>
   <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>D1</t>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>Stuff</t>
+  </si>
+  <si>
+    <t>UX100</t>
   </si>
   <si>
     <t>Touchstone Stuff</t>
@@ -109,13 +115,7 @@
     <t>Integra Luxtec Lightsource</t>
   </si>
   <si>
-    <t>Stuff</t>
-  </si>
-  <si>
     <t>Test</t>
-  </si>
-  <si>
-    <t>UX100</t>
   </si>
   <si>
     <t>New Item</t>
@@ -597,7 +597,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -645,27 +645,24 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>58</v>
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -674,12 +671,12 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -687,11 +684,8 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>35</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -704,16 +698,13 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
@@ -722,10 +713,10 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -739,10 +730,10 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -756,10 +747,10 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -773,10 +764,10 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -784,16 +775,16 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -801,19 +792,16 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -821,47 +809,41 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>28</v>
@@ -870,67 +852,64 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F16" t="s">
         <v>53</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
@@ -939,39 +918,39 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -979,13 +958,22 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" t="s">
+        <v>55</v>
+      </c>
       <c r="G20" s="2" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -998,16 +986,31 @@
       <c r="C21">
         <v>1</v>
       </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C22">
         <v>1</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1018,10 +1021,7 @@
         <v>33</v>
       </c>
       <c r="C23">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1035,27 +1035,38 @@
         <v>1</v>
       </c>
     </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G6" r:id="rId5"/>
-    <hyperlink ref="G7" r:id="rId6"/>
-    <hyperlink ref="G8" r:id="rId7"/>
-    <hyperlink ref="G9" r:id="rId8"/>
-    <hyperlink ref="G10" r:id="rId9"/>
-    <hyperlink ref="G11" r:id="rId10"/>
-    <hyperlink ref="G12" r:id="rId11"/>
-    <hyperlink ref="G13" r:id="rId12"/>
-    <hyperlink ref="G14" r:id="rId13"/>
-    <hyperlink ref="G15" r:id="rId14"/>
-    <hyperlink ref="G16" r:id="rId15"/>
-    <hyperlink ref="G17" r:id="rId16"/>
-    <hyperlink ref="G18" r:id="rId17"/>
-    <hyperlink ref="G19" r:id="rId18"/>
-    <hyperlink ref="G20" r:id="rId19"/>
+    <hyperlink ref="G4" r:id="rId1"/>
+    <hyperlink ref="G5" r:id="rId2"/>
+    <hyperlink ref="G6" r:id="rId3"/>
+    <hyperlink ref="G7" r:id="rId4"/>
+    <hyperlink ref="G8" r:id="rId5"/>
+    <hyperlink ref="G9" r:id="rId6"/>
+    <hyperlink ref="G10" r:id="rId7"/>
+    <hyperlink ref="G11" r:id="rId8"/>
+    <hyperlink ref="G12" r:id="rId9"/>
+    <hyperlink ref="G13" r:id="rId10"/>
+    <hyperlink ref="G14" r:id="rId11"/>
+    <hyperlink ref="G15" r:id="rId12"/>
+    <hyperlink ref="G16" r:id="rId13"/>
+    <hyperlink ref="G17" r:id="rId14"/>
+    <hyperlink ref="G18" r:id="rId15"/>
+    <hyperlink ref="G19" r:id="rId16"/>
+    <hyperlink ref="G20" r:id="rId17"/>
+    <hyperlink ref="G21" r:id="rId18"/>
+    <hyperlink ref="G22" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Auto-save inventory data - 2025-07-04 06:48:24
</commit_message>
<xml_diff>
--- a/inventory_data.xlsx
+++ b/inventory_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="67">
   <si>
     <t>Location</t>
   </si>
@@ -64,9 +64,6 @@
     <t>B3</t>
   </si>
   <si>
-    <t>D2</t>
-  </si>
-  <si>
     <t>Stuff</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
   </si>
   <si>
     <t>Test</t>
-  </si>
-  <si>
-    <t>New Item</t>
   </si>
   <si>
     <t>RFE2-C</t>
@@ -597,7 +591,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -640,7 +634,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -651,13 +645,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -665,13 +659,13 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -679,13 +673,13 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -693,13 +687,13 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -707,16 +701,16 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -724,16 +718,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -741,16 +735,16 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -758,16 +752,16 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -775,16 +769,16 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -792,16 +786,16 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -809,16 +803,16 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -826,19 +820,19 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -846,19 +840,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -866,22 +860,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -889,22 +883,22 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -912,22 +906,22 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -935,22 +929,22 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -958,22 +952,22 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -981,22 +975,22 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1004,13 +998,13 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1018,31 +1012,9 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto-save inventory data - 2025-07-04 06:48:34
</commit_message>
<xml_diff>
--- a/inventory_data.xlsx
+++ b/inventory_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="68">
   <si>
     <t>Location</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>16K00MLX7896</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
   <si>
     <t>System Failure, Missing Magnet</t>
@@ -665,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -679,7 +682,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -693,7 +696,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -710,7 +713,7 @@
         <v>33</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -727,7 +730,7 @@
         <v>34</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -744,7 +747,7 @@
         <v>35</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -761,7 +764,7 @@
         <v>36</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -778,7 +781,7 @@
         <v>37</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -795,7 +798,7 @@
         <v>38</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -812,7 +815,7 @@
         <v>33</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -829,10 +832,10 @@
         <v>39</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -849,10 +852,10 @@
         <v>39</v>
       </c>
       <c r="F15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -872,10 +875,10 @@
         <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -895,10 +898,10 @@
         <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -918,10 +921,10 @@
         <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -941,10 +944,10 @@
         <v>46</v>
       </c>
       <c r="F19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -964,10 +967,10 @@
         <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -987,10 +990,10 @@
         <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1004,7 +1007,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1016,6 +1019,12 @@
       </c>
       <c r="C23">
         <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-save inventory data - 2025-07-04 06:49:32
</commit_message>
<xml_diff>
--- a/inventory_data.xlsx
+++ b/inventory_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="70">
   <si>
     <t>Location</t>
   </si>
@@ -64,6 +64,9 @@
     <t>B3</t>
   </si>
   <si>
+    <t>D2</t>
+  </si>
+  <si>
     <t>Stuff</t>
   </si>
   <si>
@@ -113,6 +116,9 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>New Item</t>
   </si>
   <si>
     <t>RFE2-C</t>
@@ -594,7 +600,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -637,7 +643,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -648,13 +654,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -662,13 +668,13 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -676,13 +682,13 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -690,13 +696,13 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -704,16 +710,16 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -721,16 +727,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -738,16 +744,16 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -755,16 +761,16 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -772,16 +778,16 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -789,16 +795,16 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -806,16 +812,16 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -823,19 +829,19 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -843,19 +849,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -863,22 +869,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -886,22 +892,22 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -909,22 +915,22 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -932,22 +938,22 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F19" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -955,22 +961,22 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F20" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -978,22 +984,22 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F21" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1001,13 +1007,13 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1015,16 +1021,35 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" t="s">
-        <v>49</v>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-save inventory data - 2025-07-04 06:59:04
</commit_message>
<xml_diff>
--- a/inventory_data.xlsx
+++ b/inventory_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="67">
   <si>
     <t>Location</t>
   </si>
@@ -64,9 +64,6 @@
     <t>B3</t>
   </si>
   <si>
-    <t>D2</t>
-  </si>
-  <si>
     <t>Stuff</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>Test</t>
   </si>
   <si>
-    <t>New Item</t>
-  </si>
-  <si>
     <t>RFE2-C</t>
   </si>
   <si>
@@ -167,9 +161,6 @@
   </si>
   <si>
     <t>16K00MLX7896</t>
-  </si>
-  <si>
-    <t>123</t>
   </si>
   <si>
     <t>System Failure, Missing Magnet</t>
@@ -600,7 +591,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -643,7 +634,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -654,13 +645,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -668,13 +659,13 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -682,13 +673,13 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -696,13 +687,13 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -710,16 +701,16 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -727,16 +718,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -744,16 +735,16 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -761,16 +752,16 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -778,16 +769,16 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -795,16 +786,16 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -812,16 +803,16 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -829,19 +820,19 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -849,19 +840,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -869,22 +860,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -892,22 +883,22 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -915,22 +906,22 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -938,22 +929,22 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -961,22 +952,22 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -984,22 +975,22 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1007,13 +998,13 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1021,35 +1012,10 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23">
         <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-save inventory data - 2025-07-04 06:59:28
</commit_message>
<xml_diff>
--- a/inventory_data.xlsx
+++ b/inventory_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="68">
   <si>
     <t>Location</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>16K00MLX7896</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
   <si>
     <t>System Failure, Missing Magnet</t>
@@ -665,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -679,7 +682,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -693,7 +696,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -710,7 +713,7 @@
         <v>33</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -727,7 +730,7 @@
         <v>34</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -744,7 +747,7 @@
         <v>35</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -761,7 +764,7 @@
         <v>36</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -778,7 +781,7 @@
         <v>37</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -795,7 +798,7 @@
         <v>38</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -812,7 +815,7 @@
         <v>33</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -829,10 +832,10 @@
         <v>39</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -849,10 +852,10 @@
         <v>39</v>
       </c>
       <c r="F15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -872,10 +875,10 @@
         <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -895,10 +898,10 @@
         <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -918,10 +921,10 @@
         <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -941,10 +944,10 @@
         <v>46</v>
       </c>
       <c r="F19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -964,10 +967,10 @@
         <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -987,10 +990,10 @@
         <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1004,7 +1007,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1016,6 +1019,9 @@
       </c>
       <c r="C23">
         <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-save inventory data - 2025-07-04 06:59:50
</commit_message>
<xml_diff>
--- a/inventory_data.xlsx
+++ b/inventory_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="71">
   <si>
     <t>Location</t>
   </si>
@@ -61,6 +61,9 @@
     <t>C1</t>
   </si>
   <si>
+    <t>D2</t>
+  </si>
+  <si>
     <t>B3</t>
   </si>
   <si>
@@ -112,6 +115,9 @@
     <t>Integra Luxtec Lightsource</t>
   </si>
   <si>
+    <t>New Item</t>
+  </si>
+  <si>
     <t>Test</t>
   </si>
   <si>
@@ -143,6 +149,9 @@
   </si>
   <si>
     <t>144733</t>
+  </si>
+  <si>
+    <t>123123</t>
   </si>
   <si>
     <t>2150601326</t>
@@ -594,7 +603,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -637,7 +646,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -648,13 +657,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -662,13 +671,13 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -676,13 +685,13 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -690,13 +699,13 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -704,16 +713,16 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -721,16 +730,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -738,16 +747,16 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -755,16 +764,16 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -772,16 +781,16 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -789,16 +798,16 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -806,16 +815,16 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -823,19 +832,19 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -843,19 +852,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -863,22 +872,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F16" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -886,22 +895,22 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -909,22 +918,22 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -932,22 +941,22 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F19" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -955,22 +964,22 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F20" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -978,22 +987,22 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F21" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1001,13 +1010,10 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C22">
         <v>1</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1015,13 +1021,44 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>49</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1044,7 +1081,7 @@
     <hyperlink ref="G19" r:id="rId16"/>
     <hyperlink ref="G20" r:id="rId17"/>
     <hyperlink ref="G21" r:id="rId18"/>
-    <hyperlink ref="G22" r:id="rId19"/>
+    <hyperlink ref="G24" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>